<commit_message>
Corrected some TD that were on ft instead of meters. Rerun and MAE only drop from 64 to 58
</commit_message>
<xml_diff>
--- a/gtx/data/Duvernay/Duvernay/Duvernay well headers SPE April 21 2021 .xlsx
+++ b/gtx/data/Duvernay/Duvernay/Duvernay well headers SPE April 21 2021 .xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Geoscience\Geothermal\Datathon\Duvernay\Deliverables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProjects\gtx-2021\gtx\data\Duvernay\Duvernay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F19C85D-D72A-43E9-B718-489087F4D5B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903E0C95-9255-44EB-94BF-E37EECD7711A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10440" yWindow="-15885" windowWidth="35490" windowHeight="15015" xr2:uid="{7F6682A4-09FF-4538-BE38-49801A7F5E85}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7F6682A4-09FF-4538-BE38-49801A7F5E85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$513</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +26,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1960,7 +1966,7 @@
   <dimension ref="A1:L513"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3344,7 +3350,7 @@
         <v>13</v>
       </c>
       <c r="D37">
-        <v>12601</v>
+        <v>3840</v>
       </c>
       <c r="E37">
         <v>54.958596999999997</v>
@@ -4408,7 +4414,8 @@
         <v>13</v>
       </c>
       <c r="D65">
-        <v>7162</v>
+        <f>7162/3.281</f>
+        <v>2182.8710758914963</v>
       </c>
       <c r="E65">
         <v>51.533695000000002</v>
@@ -5700,7 +5707,7 @@
         <v>13</v>
       </c>
       <c r="D99">
-        <v>11931</v>
+        <v>3636</v>
       </c>
       <c r="E99">
         <v>54.685861000000003</v>
@@ -5890,7 +5897,8 @@
         <v>13</v>
       </c>
       <c r="D104">
-        <v>7244</v>
+        <f>7244/3.281</f>
+        <v>2207.8634562633342</v>
       </c>
       <c r="E104">
         <v>52.279187999999998</v>
@@ -6384,7 +6392,8 @@
         <v>13</v>
       </c>
       <c r="D117">
-        <v>7241.1</v>
+        <f>7241.1/3.281</f>
+        <v>2206.9795793965254</v>
       </c>
       <c r="E117">
         <v>52.148497999999996</v>
@@ -6422,7 +6431,8 @@
         <v>13</v>
       </c>
       <c r="D118">
-        <v>7795</v>
+        <f>7795/3.281</f>
+        <v>2375.8000609570254</v>
       </c>
       <c r="E118">
         <v>51.868988000000002</v>
@@ -6650,7 +6660,8 @@
         <v>13</v>
       </c>
       <c r="D124">
-        <v>7281</v>
+        <f>7281/3.281</f>
+        <v>2219.14050594331</v>
       </c>
       <c r="E124">
         <v>51.788694</v>
@@ -6764,7 +6775,8 @@
         <v>13</v>
       </c>
       <c r="D127">
-        <v>8775</v>
+        <f>8775/3.281</f>
+        <v>2674.489484913136</v>
       </c>
       <c r="E127">
         <v>53.139642000000002</v>
@@ -7524,7 +7536,8 @@
         <v>13</v>
       </c>
       <c r="D147">
-        <v>7549</v>
+        <f>7549/3.281</f>
+        <v>2300.8229198415115</v>
       </c>
       <c r="E147">
         <v>52.097197999999999</v>
@@ -7600,7 +7613,8 @@
         <v>13</v>
       </c>
       <c r="D149">
-        <v>8668</v>
+        <f>8668/3.281</f>
+        <v>2641.8774763791525</v>
       </c>
       <c r="E149">
         <v>51.920161</v>
@@ -7866,7 +7880,8 @@
         <v>13</v>
       </c>
       <c r="D156">
-        <v>7224.1</v>
+        <f>7224.1/3.281</f>
+        <v>2201.7982322462663</v>
       </c>
       <c r="E156">
         <v>51.789017999999999</v>
@@ -7980,7 +7995,8 @@
         <v>13</v>
       </c>
       <c r="D159">
-        <v>8345</v>
+        <f>8345/3.281</f>
+        <v>2543.4318805242301</v>
       </c>
       <c r="E159">
         <v>51.632565999999997</v>
@@ -8208,7 +8224,8 @@
         <v>13</v>
       </c>
       <c r="D165">
-        <v>8290</v>
+        <f>8290/3.281</f>
+        <v>2526.6686985675096</v>
       </c>
       <c r="E165">
         <v>52.750681999999998</v>
@@ -8968,7 +8985,7 @@
         <v>13</v>
       </c>
       <c r="D185">
-        <v>11832</v>
+        <v>3603</v>
       </c>
       <c r="E185">
         <v>52.452556000000001</v>
@@ -9424,7 +9441,8 @@
         <v>13</v>
       </c>
       <c r="D197">
-        <v>13600.1</v>
+        <f>13600.1/3.281</f>
+        <v>4145.1081987199022</v>
       </c>
       <c r="E197">
         <v>52.601562999999999</v>
@@ -9538,7 +9556,8 @@
         <v>13</v>
       </c>
       <c r="D200">
-        <v>13109</v>
+        <f>13109/3.281</f>
+        <v>3995.4282231027123</v>
       </c>
       <c r="E200">
         <v>52.459530000000001</v>
@@ -9842,7 +9861,8 @@
         <v>13</v>
       </c>
       <c r="D208">
-        <v>13157.2</v>
+        <f>13157.2/3.281</f>
+        <v>4010.1188661993297</v>
       </c>
       <c r="E208">
         <v>53.756720000000001</v>
@@ -21460,6 +21480,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L513" xr:uid="{AF2C3E19-358C-4018-BED2-AC47DEE09945}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>